<commit_message>
Updated Check Doc and added Discrepancy found
</commit_message>
<xml_diff>
--- a/Data/Testdata.xlsx
+++ b/Data/Testdata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Unique\git\Trade_EE_Application\Trade_EE_Application\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BDD Cucumber Prj\Trade_EE_Application2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{603C31F1-EBD8-4FF8-8864-418B69AC8837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FCD02F-2335-49E9-BA4E-038A064FCF66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{375EF1B1-9957-4315-AB63-D4C2E84C70EB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{375EF1B1-9957-4315-AB63-D4C2E84C70EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,8 @@
     <sheet name="IssueLC" sheetId="4" r:id="rId3"/>
     <sheet name="RegAmend" sheetId="5" r:id="rId4"/>
     <sheet name="RegDoc" sheetId="6" r:id="rId5"/>
-    <sheet name="Calc" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId6"/>
+    <sheet name="Calc" sheetId="3" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="113">
   <si>
     <t>Business Unit</t>
   </si>
@@ -358,6 +359,18 @@
   </si>
   <si>
     <t>Beneficiary</t>
+  </si>
+  <si>
+    <t>DOC_STATUS</t>
+  </si>
+  <si>
+    <t>Compliant</t>
+  </si>
+  <si>
+    <t>DISC_NOTED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Message to be covered. </t>
   </si>
 </sst>
 </file>
@@ -845,7 +858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2689149-262B-4103-A4F5-B0F1843BF906}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
@@ -1147,7 +1160,7 @@
       </c>
       <c r="D2" s="3">
         <f ca="1">TODAY()</f>
-        <v>45902</v>
+        <v>45908</v>
       </c>
       <c r="E2" t="str">
         <f>RegisterLC!C2</f>
@@ -1378,10 +1391,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D45EB6AE-18D4-4CDC-AC7D-04A6C2F4F441}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1399,9 +1412,11 @@
     <col min="14" max="14" width="20.21875" customWidth="1"/>
     <col min="15" max="15" width="14.6640625" customWidth="1"/>
     <col min="16" max="16" width="23.21875" customWidth="1"/>
+    <col min="17" max="17" width="30.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>91</v>
       </c>
@@ -1450,8 +1465,14 @@
       <c r="P1" s="15" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="Q1" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="R1" s="15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2500</v>
       </c>
@@ -1491,11 +1512,20 @@
       <c r="P2" t="s">
         <v>108</v>
       </c>
+      <c r="Q2" t="s">
+        <v>110</v>
+      </c>
+      <c r="R2" t="s">
+        <v>112</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2" xr:uid="{407D7200-94FB-4703-8610-6010850128D9}">
       <formula1>"Beneficiary, Advising Bank, Advise Through Bank"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2" xr:uid="{E3E4FA39-9706-409B-99D6-D758E6D1D734}">
+      <formula1>"Compliant, Discrepancy Found, Under Shipping Guarantee, Goods Released Already, Accepted by Applicant as Presented"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1504,6 +1534,18 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC3EC9D4-5259-4CF9-A600-70073945E2F1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D71899EE-AB73-493C-A489-80FA5D741168}">
   <dimension ref="A1:F18"/>
   <sheetViews>

</xml_diff>

<commit_message>
Latest update on settlement and issue LC
</commit_message>
<xml_diff>
--- a/Data/Testdata.xlsx
+++ b/Data/Testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BDD Cucumber Prj\Trade_EE_Application2\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0867579F-F0D6-488E-B500-6FF4996EBE47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CFB41AF-E800-48D4-BCF9-B6E1752A6810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{375EF1B1-9957-4315-AB63-D4C2E84C70EB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{375EF1B1-9957-4315-AB63-D4C2E84C70EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="116">
   <si>
     <t>Business Unit</t>
   </si>
@@ -241,9 +241,6 @@
     <t>PERCEN</t>
   </si>
   <si>
-    <t>BY MIXED PYMT</t>
-  </si>
-  <si>
     <t>MIX_TENOR_DAYS</t>
   </si>
   <si>
@@ -374,6 +371,15 @@
   </si>
   <si>
     <t>TENOR_DT</t>
+  </si>
+  <si>
+    <t>CHARGES_ACC</t>
+  </si>
+  <si>
+    <t>By Payment</t>
+  </si>
+  <si>
+    <t>DRAWEE_ID</t>
   </si>
 </sst>
 </file>
@@ -861,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2689149-262B-4103-A4F5-B0F1843BF906}">
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -960,7 +966,7 @@
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>114</v>
       </c>
       <c r="D2" t="s">
         <v>40</v>
@@ -1035,10 +1041,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1E9E443-5901-4CA5-8075-A94B47B41018}">
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="Z13" sqref="Z13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1066,9 +1072,10 @@
     <col min="23" max="23" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="24" max="25" width="16.109375" customWidth="1"/>
     <col min="26" max="26" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -1133,10 +1140,10 @@
         <v>68</v>
       </c>
       <c r="V1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="W1" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="X1" s="2" t="s">
         <v>28</v>
@@ -1145,10 +1152,13 @@
         <v>29</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>RegisterLC!A2</f>
         <v>IRREVOCABLE</v>
@@ -1163,11 +1173,11 @@
       </c>
       <c r="D2" s="3">
         <f ca="1">TODAY()</f>
-        <v>45917</v>
+        <v>45935</v>
       </c>
       <c r="E2" t="str">
         <f>RegisterLC!C2</f>
-        <v>BY MIXED PYMT</v>
+        <v>By Payment</v>
       </c>
       <c r="F2" t="str">
         <f>RegisterLC!D2</f>
@@ -1201,7 +1211,7 @@
       </c>
       <c r="O2" t="str">
         <f>RegisterLC!C2</f>
-        <v>BY MIXED PYMT</v>
+        <v>By Payment</v>
       </c>
       <c r="P2" t="s">
         <v>58</v>
@@ -1216,7 +1226,7 @@
         <v>66</v>
       </c>
       <c r="T2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="U2">
         <v>60</v>
@@ -1238,6 +1248,9 @@
       <c r="Z2">
         <f>RegisterLC!V2</f>
         <v>123456789</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1289,46 +1302,46 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>75</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>14</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>79</v>
-      </c>
       <c r="H1" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="J1" s="7" t="s">
-        <v>83</v>
-      </c>
       <c r="K1" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="L1" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="M1" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="M1" s="7" t="s">
-        <v>87</v>
-      </c>
       <c r="N1" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
@@ -1349,13 +1362,13 @@
         <v>3675</v>
       </c>
       <c r="G2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I2">
         <v>5</v>
       </c>
       <c r="J2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K2" t="s">
         <v>52</v>
@@ -1364,10 +1377,10 @@
         <v>58</v>
       </c>
       <c r="M2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="N2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
@@ -1421,58 +1434,58 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>92</v>
-      </c>
       <c r="C1" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="K1" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="L1" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="P1" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="G1" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>98</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="L1" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="N1" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="O1" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="P1" s="15" t="s">
-        <v>107</v>
-      </c>
       <c r="Q1" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="R1" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -1480,7 +1493,7 @@
         <v>2500</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -1513,13 +1526,13 @@
         <v>2</v>
       </c>
       <c r="P2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="Q2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>
@@ -1538,26 +1551,47 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC3EC9D4-5259-4CF9-A600-70073945E2F1}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <f ca="1">TODAY()</f>
-        <v>45917</v>
+        <v>45935</v>
+      </c>
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2">
+        <v>56555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>